<commit_message>
Updated the changes on flow
</commit_message>
<xml_diff>
--- a/src/main/java/com/app/qa/testdata/ArriveCANData.xlsx
+++ b/src/main/java/com/app/qa/testdata/ArriveCANData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albinjoy/Documents/development/ArriveCAN/src/main/java/com/app/qa/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\ArriveCAN\src\main\java\com\app\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B207466C-C993-8647-BA92-D5F8719CBFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B7A5DD-D468-473C-8FC6-A03EC5E2F090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="arrivecan" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>title</t>
   </si>
@@ -84,51 +84,15 @@
     <t>TestCase</t>
   </si>
   <si>
-    <t>TravelPurp_btn</t>
-  </si>
-  <si>
     <t>TravelPurp_lbl</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Cross-border work</t>
-  </si>
-  <si>
     <t>Entry_Type</t>
   </si>
   <si>
     <t>air</t>
   </si>
   <si>
-    <t>Traveller_doctype</t>
-  </si>
-  <si>
-    <t>Traveller_surname</t>
-  </si>
-  <si>
-    <t>Traveller_givename</t>
-  </si>
-  <si>
-    <t>Traveller_dob</t>
-  </si>
-  <si>
-    <t>US Permanent Resident Card</t>
-  </si>
-  <si>
-    <t>Traveller_docnum</t>
-  </si>
-  <si>
-    <t>5647835784358</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Eric</t>
-  </si>
-  <si>
     <t>Traveller_mobile</t>
   </si>
   <si>
@@ -138,9 +102,6 @@
     <t>France</t>
   </si>
   <si>
-    <t>1960-10-01</t>
-  </si>
-  <si>
     <t>4162156789</t>
   </si>
   <si>
@@ -169,6 +130,15 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Work/employment or essential reasons  &amp;&amp; Cross-border worker</t>
+  </si>
+  <si>
+    <t>selectTraveller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jane Doe </t>
   </si>
 </sst>
 </file>
@@ -504,28 +474,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ED45E7-CFC1-AC48-9C04-4ECF0D26B37E}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -536,145 +501,85 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G4" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -690,9 +595,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -720,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -734,7 +639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -759,7 +664,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -771,7 +676,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated handling if no traveller is found
</commit_message>
<xml_diff>
--- a/src/main/java/com/app/qa/testdata/ArriveCANData.xlsx
+++ b/src/main/java/com/app/qa/testdata/ArriveCANData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\ArriveCAN\src\main\java\com\app\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B7A5DD-D468-473C-8FC6-A03EC5E2F090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9957586D-0515-48F6-99BF-86B853793599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>title</t>
   </si>
@@ -132,13 +132,43 @@
     <t>3</t>
   </si>
   <si>
-    <t xml:space="preserve">  Work/employment or essential reasons  &amp;&amp; Cross-border worker</t>
-  </si>
-  <si>
     <t>selectTraveller</t>
   </si>
   <si>
     <t xml:space="preserve"> Jane Doe </t>
+  </si>
+  <si>
+    <t>Traveller_doctype</t>
+  </si>
+  <si>
+    <t>Traveller_docnum</t>
+  </si>
+  <si>
+    <t>Traveller_surname</t>
+  </si>
+  <si>
+    <t>Traveller_givename</t>
+  </si>
+  <si>
+    <t>Traveller_dob</t>
+  </si>
+  <si>
+    <t>US Permanent Resident Card</t>
+  </si>
+  <si>
+    <t>5647835784358</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>2020-10-01</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Cross-border worker</t>
   </si>
 </sst>
 </file>
@@ -474,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ED45E7-CFC1-AC48-9C04-4ECF0D26B37E}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -490,7 +520,7 @@
     <col min="6" max="6" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -501,7 +531,7 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>20</v>
@@ -512,19 +542,34 @@
       <c r="G1" t="s">
         <v>30</v>
       </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -535,19 +580,34 @@
       <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
@@ -558,19 +618,34 @@
       <c r="G3" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -580,6 +655,21 @@
       </c>
       <c r="G4" s="4" t="s">
         <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added synchronization wait concept
</commit_message>
<xml_diff>
--- a/src/main/java/com/app/qa/testdata/ArriveCANData.xlsx
+++ b/src/main/java/com/app/qa/testdata/ArriveCANData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\ArriveCAN\src\main\java\com\app\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9957586D-0515-48F6-99BF-86B853793599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DB4CAB-16E4-438E-B1EF-B1D87EE150CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,19 @@
     <sheet name="deals" sheetId="2" r:id="rId3"/>
     <sheet name="tasks" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="74">
   <si>
     <t>title</t>
   </si>
@@ -105,15 +114,6 @@
     <t>4162156789</t>
   </si>
   <si>
-    <t>createExempt_air</t>
-  </si>
-  <si>
-    <t>createExempt_land</t>
-  </si>
-  <si>
-    <t>createExempt_marine</t>
-  </si>
-  <si>
     <t>IGNORE</t>
   </si>
   <si>
@@ -169,6 +169,99 @@
   </si>
   <si>
     <t>Work/employment or essential reasons  &amp;&amp; Cross-border worker</t>
+  </si>
+  <si>
+    <t>Cross-border worker_air</t>
+  </si>
+  <si>
+    <t>Cross-border worker_land</t>
+  </si>
+  <si>
+    <t>Cross-border worker_marine</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Trade or transport</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Performance of other essential services</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Other medical services or care</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Marine transportation sector</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Crossing to and from border communities for everyday functions (including school)</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Performance of specific essential services</t>
+  </si>
+  <si>
+    <t>Work/employment or essential reasons  &amp;&amp; Essential medical services, transport or deliveries</t>
+  </si>
+  <si>
+    <t>Trade or transport_air</t>
+  </si>
+  <si>
+    <t>Trade or transport_land</t>
+  </si>
+  <si>
+    <t>Trade or transport_marine</t>
+  </si>
+  <si>
+    <t>Performance of other essential services_air</t>
+  </si>
+  <si>
+    <t>Performance of other essential services_land</t>
+  </si>
+  <si>
+    <t>Performance of other essential services_marine</t>
+  </si>
+  <si>
+    <t>Other medical services or care_air</t>
+  </si>
+  <si>
+    <t>Other medical services or care_land</t>
+  </si>
+  <si>
+    <t>Other medical services or care_marine</t>
+  </si>
+  <si>
+    <t>Marine transportation sector_air</t>
+  </si>
+  <si>
+    <t>Marine transportation sector_land</t>
+  </si>
+  <si>
+    <t>Marine transportation sector_marine</t>
+  </si>
+  <si>
+    <t>Crossing to and from border communities for everyday functions (including school)_air</t>
+  </si>
+  <si>
+    <t>Crossing to and from border communities for everyday functions (including school)_land</t>
+  </si>
+  <si>
+    <t>Crossing to and from border communities for everyday functions (including school)_marine</t>
+  </si>
+  <si>
+    <t>Performance of specific essential services_air</t>
+  </si>
+  <si>
+    <t>Performance of specific essential services_land</t>
+  </si>
+  <si>
+    <t>Performance of specific essential services_marine</t>
+  </si>
+  <si>
+    <t>Essential medical services, transport or deliveries_air</t>
+  </si>
+  <si>
+    <t>Essential medical services, transport or deliveries_land</t>
+  </si>
+  <si>
+    <t>Essential medical services, transport or deliveries_marine</t>
   </si>
 </sst>
 </file>
@@ -504,15 +597,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ED45E7-CFC1-AC48-9C04-4ECF0D26B37E}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.625" bestFit="1" customWidth="1"/>
@@ -521,55 +614,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -578,74 +671,74 @@
         <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -654,22 +747,820 @@
         <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" t="s">
+        <v>40</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K22" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" t="s">
+        <v>40</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>